<commit_message>
hours and moved stuff
</commit_message>
<xml_diff>
--- a/hours/Hours.xlsx
+++ b/hours/Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="209">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -905,10 +905,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I246"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A220" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E247" activeCellId="0" sqref="E247"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A226" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A248" activeCellId="0" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -969,7 +969,7 @@
       </c>
       <c r="G2" s="4" t="n">
         <f aca="true">CEILING(NOW()-A124, 1)</f>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H2" s="5" t="n">
         <f aca="false">(SUM(D218:D240))*24</f>
@@ -977,7 +977,7 @@
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">H2/(G2*24)</f>
-        <v>0.00580929487179487</v>
+        <v>0.00577229299363057</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5431,6 +5431,24 @@
         <v>0.03125</v>
       </c>
       <c r="E246" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B247" s="2" t="n">
+        <v>0.357638888888889</v>
+      </c>
+      <c r="C247" s="2" t="n">
+        <v>0.388888888888889</v>
+      </c>
+      <c r="D247" s="3" t="n">
+        <f aca="false">C247-B247</f>
+        <v>0.03125</v>
+      </c>
+      <c r="E247" s="0" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>